<commit_message>
Deleted the polygon and polyhedron classes
Created the shape class to take their places. The shape class
will have all the necessary volume and area calcs and will be
able to perform those calcs on any shape  or portion of a shape
by moving the pointer to its base data array.
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -32,6 +32,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -120,7 +121,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -301,6 +302,10 @@
         <f aca="false">D3-$D$7</f>
         <v>2.98875</v>
       </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">5/6</f>
+        <v>0.833333333333333</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -317,6 +322,10 @@
       <c r="D13" s="0" t="n">
         <f aca="false">D4-$D$7</f>
         <v>5.28875</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">72/6</f>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,6 +344,16 @@
       <c r="D14" s="0" t="n">
         <f aca="false">D10</f>
         <v>-2.98625</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">144/6</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="0" t="n">
+        <f aca="false">1/12</f>
+        <v>0.0833333333333333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added the Quad area function.
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -118,10 +118,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -235,6 +235,24 @@
         <v>15.395</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="n">
+        <f aca="false">(B4-B2)^2</f>
+        <v>82.2649</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">(C4-C2)^2</f>
+        <v>5.9049</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">(D4-D2)^2</f>
+        <v>111.9364</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">SQRT(SUM(F6:H6) )</f>
+        <v>14.14588986243</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>0</v>
@@ -442,6 +460,88 @@
       <c r="D25" s="0" t="n">
         <f aca="false">0.5*D23</f>
         <v>51.210665</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <f aca="false">B1-B3</f>
+        <v>9.325</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">C1-C3</f>
+        <v>8.794</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">D1-D3</f>
+        <v>-5.975</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <f aca="false">B2-B4</f>
+        <v>-9.07</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">C2-C4</f>
+        <v>2.43</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">D2-D4</f>
+        <v>-10.58</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <f aca="false">C28*D29-D28*C29</f>
+        <v>-78.52127</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">D28*B29-B28*D29</f>
+        <v>152.85175</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">B28*C29-C28*B29</f>
+        <v>102.42133</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">SQRT(B32^2+C32^2+D32^2)/2</f>
+        <v>100.024217266925</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <f aca="false">B1-B2</f>
+        <v>9.197</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">C1-C2</f>
+        <v>3.183</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">D1-D2</f>
+        <v>2.305</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">B34*B32+C34*C32+D34*D32</f>
+        <v>0.448165709999955</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="n">
+        <f aca="false">B3-B4</f>
+        <v>-9.198</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">C3-C4</f>
+        <v>-3.181</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">D3-D4</f>
+        <v>-2.3</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">B36*B32+C36*C32+D36*D32</f>
+        <v>0.448165710000012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in Vect operator+= and added VolPyra and VolPrism
The volume calcs are based on a degenerate hex volume. The
operator+= in Vect was mistyped as operator+
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -5,19 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>centroid</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -120,7 +127,7 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -553,4 +560,312 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B8:E37"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <f aca="false">B8+1</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <f aca="false">B9+1</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <f aca="false">B10+1</f>
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <f aca="false">B11+1</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <f aca="false">B12+1</f>
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <f aca="false">B13+1</f>
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <f aca="false">B14+1</f>
+        <v>7</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="n">
+        <f aca="false">C14-C9+C15-C8</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">D14-D9+D15-D8</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">E14-E9+E15-E8</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">C14-C11</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">D14-D11</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">E14-E11</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="false">C10-C8</f>
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">D10-D8</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">E10-E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <f aca="false">(D19*E20-E19*D20)*C18+(E19*C20-C19*E20)*D18+(C19*D20-D19*C20)*E18</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <f aca="false">C15-C8</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">D15-D8</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">E15-E8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="n">
+        <f aca="false">C14-C11+C13-C8</f>
+        <v>4</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">D14-D11+D13-D8</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">E14-E11+E13-E8</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="n">
+        <f aca="false">C14-C12</f>
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">D14-D12</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">E14-E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="n">
+        <f aca="false">(D25*E26-D26*E25)*C24-(C25*E26-C26*E25)*D24+(C25*D26-C26*D25)*E24</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="n">
+        <f aca="false">C14-C9</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">D14-D9</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">E14-E9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="n">
+        <f aca="false">C13-C8</f>
+        <v>2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">D13-D8</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">E13-E8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="n">
+        <f aca="false">C14-C12+C10-C8</f>
+        <v>4</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">D14-D12+D10-D8</f>
+        <v>2</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">E14-E12+E10-E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="n">
+        <f aca="false">(D31*E32-D32*E31)*C30-(C31*E32-C32*E31)*D30+(C31*D32-C32*D31)*E30</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <f aca="false">C22+C28+C34</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="n">
+        <f aca="false">C36/12</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added distance formula to point.
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -127,8 +128,8 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -569,7 +570,7 @@
   </sheetPr>
   <dimension ref="B8:E37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -868,4 +869,71 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>9.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <f aca="false">(A2-A1)^2</f>
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">(B2-B1)^2</f>
+        <v>42.25</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">(C2-C1)^2</f>
+        <v>39.69</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">SQRT(SUM(A4:C4))</f>
+        <v>9.89646401499041</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated hermite spline a little and added node class
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,19 +13,24 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>centroid</t>
+    <t xml:space="preserve">centroid</t>
   </si>
   <si>
-    <t>a</t>
+    <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t>b</t>
+    <t xml:space="preserve">b</t>
   </si>
 </sst>
 </file>
@@ -33,7 +38,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -133,9 +138,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -575,9 +577,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
@@ -876,16 +875,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -925,6 +921,83 @@
       <c r="E4" s="0" t="n">
         <f aca="false">SQRT(SUM(A4:C4))</f>
         <v>9.89646401499041</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">SQRT(4-A11^2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <f aca="false">A11+0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">SQRT(4-A12^2)</f>
+        <v>1.95959179422654</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <f aca="false">A12+0.4</f>
+        <v>0.8</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">SQRT(4-A13^2)</f>
+        <v>1.83303027798234</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <f aca="false">A13+0.4</f>
+        <v>1.2</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">SQRT(4-A14^2)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <f aca="false">A14+0.4</f>
+        <v>1.6</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">SQRT(4-A15^2)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <f aca="false">A15+0.4</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">SQRT(4-A16^2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <f aca="false">2*SIN(PI()/4)</f>
+        <v>1.4142135623731</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <f aca="false">2*COS(PI()/4)</f>
+        <v>1.4142135623731</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <f aca="false">PI()*4/4</f>
+        <v>3.14159265358979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a concrete curve class and line class
Tested hermite spline and created a common concnrete class for all
curves to derive from.
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -40,7 +40,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -61,6 +61,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,13 +110,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -138,6 +147,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -577,6 +589,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
@@ -875,13 +890,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -923,6 +941,79 @@
         <v>9.89646401499041</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <f aca="false">PI()/8</f>
+        <v>0.392699081698724</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">2*COS(I6*$H$6)</f>
+        <v>2</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <f aca="false">2*SIN(I6*$H$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="0" t="n">
+        <f aca="false">I6+1</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">2*COS(I7*$H$6)</f>
+        <v>1.84775906502257</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <f aca="false">2*SIN(I7*$H$6)</f>
+        <v>0.76536686473018</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="0" t="n">
+        <f aca="false">I7+1</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">2*COS(I8*$H$6)</f>
+        <v>1.4142135623731</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <f aca="false">2*SIN(I8*$H$6)</f>
+        <v>1.4142135623731</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="0" t="n">
+        <f aca="false">I8+1</f>
+        <v>3</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">2*COS(I9*$H$6)</f>
+        <v>0.76536686473018</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <f aca="false">2*SIN(I9*$H$6)</f>
+        <v>1.84775906502257</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="0" t="n">
+        <f aca="false">I9+1</f>
+        <v>4</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">2*COS(I10*$H$6)</f>
+        <v>1.22464679914735E-016</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <f aca="false">2*SIN(I10*$H$6)</f>
+        <v>2</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>0</v>
@@ -930,6 +1021,9 @@
       <c r="B11" s="0" t="n">
         <f aca="false">SQRT(4-A11^2)</f>
         <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,6 +1035,18 @@
         <f aca="false">SQRT(4-A12^2)</f>
         <v>1.95959179422654</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">SQRT((A12-A11)^2+(B12-B11)^2)</f>
+        <v>0.402035848020833</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">D12</f>
+        <v>0.402035848020833</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">E12/PI()</f>
+        <v>0.127971985025315</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -951,6 +1057,18 @@
         <f aca="false">SQRT(4-A13^2)</f>
         <v>1.83303027798234</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">SQRT((A13-A12)^2+(B13-B12)^2)</f>
+        <v>0.419544774003956</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">E12+D13</f>
+        <v>0.821580622024789</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">E13/PI()</f>
+        <v>0.261517234287519</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -961,6 +1079,18 @@
         <f aca="false">SQRT(4-A14^2)</f>
         <v>1.6</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">SQRT((A14-A13)^2+(B14-B13)^2)</f>
+        <v>0.462928839516968</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">E13+D14</f>
+        <v>1.28450946154176</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">E14/PI()</f>
+        <v>0.408872060505359</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -971,6 +1101,18 @@
         <f aca="false">SQRT(4-A15^2)</f>
         <v>1.2</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">SQRT((A15-A14)^2+(B15-B14)^2)</f>
+        <v>0.565685424949238</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">E14+D15</f>
+        <v>1.850194886491</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">E15/PI()</f>
+        <v>0.58893532373678</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -980,6 +1122,18 @@
       <c r="B16" s="0" t="n">
         <f aca="false">SQRT(4-A16^2)</f>
         <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">SQRT((A16-A15)^2+(B16-B15)^2)</f>
+        <v>1.26491106406735</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">E15+D16</f>
+        <v>3.11510595055835</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">E16/PI()</f>
+        <v>0.991569020572677</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,6 +1141,10 @@
         <f aca="false">2*SIN(PI()/4)</f>
         <v>1.4142135623731</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">(1.444-A18)/A18</f>
+        <v>0.021062192033371</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -998,6 +1156,24 @@
       <c r="A21" s="0" t="n">
         <f aca="false">PI()*4/4</f>
         <v>3.14159265358979</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <f aca="false">SQRT(2)</f>
+        <v>1.4142135623731</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="n">
+        <f aca="false">0.25-0.128</f>
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="0" t="n">
+        <f aca="false">E24*3.1415</f>
+        <v>0.383263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started implementing surfaceI and surface
</commit_message>
<xml_diff>
--- a/geom/UnitTests/excel/calcs.xlsx
+++ b/geom/UnitTests/excel/calcs.xlsx
@@ -893,7 +893,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1163,6 +1163,14 @@
         <f aca="false">SQRT(2)</f>
         <v>1.4142135623731</v>
       </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">0.25*1+0.75*4</f>
+        <v>3.25</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">0.25*1+0.75*3</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="0" t="n">

</xml_diff>